<commit_message>
fix SLR_table to parse LHS
</commit_message>
<xml_diff>
--- a/SLR_table.xlsx
+++ b/SLR_table.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10312"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10514"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/eomchanwoo/CP_PROJECT/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sseungwonnn/git/CP_PROJECT/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E893F1F-47B8-B34B-B2A6-6B00CFC58B60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2966D670-57BA-1847-9D1C-C11E51ED1F1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="14400" windowHeight="17500" activeTab="1" xr2:uid="{DE6245F0-BCA7-4240-8F6E-8ABD7213D53C}"/>
   </bookViews>
@@ -6800,8 +6800,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D1ECCCD-2683-9B43-BA07-36C0A247F203}">
   <dimension ref="A1:F40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="106" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="106" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18"/>
@@ -6841,8 +6841,8 @@
         <v>164</v>
       </c>
       <c r="C2" s="19" t="str">
-        <f>LEFT(B2,F2)</f>
-        <v xml:space="preserve">S' </v>
+        <f>LEFT(B2,F2-1)</f>
+        <v>S'</v>
       </c>
       <c r="D2" s="22" t="str">
         <f>RIGHT(B2,LEN(B2)-F2-3)</f>
@@ -6865,8 +6865,8 @@
         <v>171</v>
       </c>
       <c r="C3" s="20" t="str">
-        <f>LEFT(B3,F3)</f>
-        <v xml:space="preserve">CODE </v>
+        <f>LEFT(B3,F3-1)</f>
+        <v>CODE</v>
       </c>
       <c r="D3" s="23" t="str">
         <f t="shared" ref="D3:D40" si="0">RIGHT(B3,LEN(B3)-F3-3)</f>
@@ -6889,8 +6889,8 @@
         <v>128</v>
       </c>
       <c r="C4" s="20" t="str">
-        <f t="shared" ref="C4:C40" si="3">LEFT(B4,F4)</f>
-        <v xml:space="preserve">CODE </v>
+        <f t="shared" ref="C4:C40" si="3">LEFT(B4,F4-1)</f>
+        <v>CODE</v>
       </c>
       <c r="D4" s="23" t="str">
         <f t="shared" si="0"/>
@@ -6914,7 +6914,7 @@
       </c>
       <c r="C5" s="20" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">CODE </v>
+        <v>CODE</v>
       </c>
       <c r="D5" s="23" t="str">
         <f t="shared" si="0"/>
@@ -6938,7 +6938,7 @@
       </c>
       <c r="C6" s="20" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">CODE </v>
+        <v>CODE</v>
       </c>
       <c r="D6" s="23" t="str">
         <f t="shared" si="0"/>
@@ -6962,7 +6962,7 @@
       </c>
       <c r="C7" s="20" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">VDECL </v>
+        <v>VDECL</v>
       </c>
       <c r="D7" s="23" t="str">
         <f t="shared" si="0"/>
@@ -6986,7 +6986,7 @@
       </c>
       <c r="C8" s="20" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">VDECL </v>
+        <v>VDECL</v>
       </c>
       <c r="D8" s="23" t="str">
         <f t="shared" si="0"/>
@@ -7010,7 +7010,7 @@
       </c>
       <c r="C9" s="20" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">ASSIGN </v>
+        <v>ASSIGN</v>
       </c>
       <c r="D9" s="23" t="str">
         <f t="shared" si="0"/>
@@ -7034,7 +7034,7 @@
       </c>
       <c r="C10" s="20" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">RHS </v>
+        <v>RHS</v>
       </c>
       <c r="D10" s="23" t="str">
         <f t="shared" si="0"/>
@@ -7058,7 +7058,7 @@
       </c>
       <c r="C11" s="20" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">RHS </v>
+        <v>RHS</v>
       </c>
       <c r="D11" s="23" t="str">
         <f t="shared" si="0"/>
@@ -7082,7 +7082,7 @@
       </c>
       <c r="C12" s="20" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">RHS </v>
+        <v>RHS</v>
       </c>
       <c r="D12" s="23" t="str">
         <f t="shared" si="0"/>
@@ -7106,7 +7106,7 @@
       </c>
       <c r="C13" s="20" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">RHS </v>
+        <v>RHS</v>
       </c>
       <c r="D13" s="23" t="str">
         <f t="shared" si="0"/>
@@ -7130,7 +7130,7 @@
       </c>
       <c r="C14" s="20" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">EXPR </v>
+        <v>EXPR</v>
       </c>
       <c r="D14" s="23" t="str">
         <f t="shared" si="0"/>
@@ -7154,7 +7154,7 @@
       </c>
       <c r="C15" s="20" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">EXPR </v>
+        <v>EXPR</v>
       </c>
       <c r="D15" s="23" t="str">
         <f t="shared" si="0"/>
@@ -7178,7 +7178,7 @@
       </c>
       <c r="C16" s="20" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">EXPR </v>
+        <v>EXPR</v>
       </c>
       <c r="D16" s="23" t="str">
         <f t="shared" si="0"/>
@@ -7202,7 +7202,7 @@
       </c>
       <c r="C17" s="20" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">EXPR’ </v>
+        <v>EXPR’</v>
       </c>
       <c r="D17" s="23" t="str">
         <f t="shared" si="0"/>
@@ -7226,7 +7226,7 @@
       </c>
       <c r="C18" s="20" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">EXPR’ </v>
+        <v>EXPR’</v>
       </c>
       <c r="D18" s="23" t="str">
         <f t="shared" si="0"/>
@@ -7250,7 +7250,7 @@
       </c>
       <c r="C19" s="20" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">EXPR’ </v>
+        <v>EXPR’</v>
       </c>
       <c r="D19" s="23" t="str">
         <f t="shared" si="0"/>
@@ -7274,7 +7274,7 @@
       </c>
       <c r="C20" s="20" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">FDECL </v>
+        <v>FDECL</v>
       </c>
       <c r="D20" s="23" t="str">
         <f t="shared" si="0"/>
@@ -7298,7 +7298,7 @@
       </c>
       <c r="C21" s="20" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">ARG </v>
+        <v>ARG</v>
       </c>
       <c r="D21" s="23" t="str">
         <f t="shared" si="0"/>
@@ -7322,7 +7322,7 @@
       </c>
       <c r="C22" s="20" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">ARG </v>
+        <v>ARG</v>
       </c>
       <c r="D22" s="23" t="str">
         <f t="shared" si="0"/>
@@ -7346,7 +7346,7 @@
       </c>
       <c r="C23" s="20" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">MOREARGS </v>
+        <v>MOREARGS</v>
       </c>
       <c r="D23" s="23" t="str">
         <f t="shared" si="0"/>
@@ -7370,7 +7370,7 @@
       </c>
       <c r="C24" s="20" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">MOREARGS </v>
+        <v>MOREARGS</v>
       </c>
       <c r="D24" s="23" t="str">
         <f t="shared" si="0"/>
@@ -7394,7 +7394,7 @@
       </c>
       <c r="C25" s="20" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">BLOCK </v>
+        <v>BLOCK</v>
       </c>
       <c r="D25" s="23" t="str">
         <f t="shared" si="0"/>
@@ -7418,7 +7418,7 @@
       </c>
       <c r="C26" s="20" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">BLOCK </v>
+        <v>BLOCK</v>
       </c>
       <c r="D26" s="23" t="str">
         <f t="shared" si="0"/>
@@ -7442,7 +7442,7 @@
       </c>
       <c r="C27" s="20" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">STMT </v>
+        <v>STMT</v>
       </c>
       <c r="D27" s="23" t="str">
         <f t="shared" si="0"/>
@@ -7466,7 +7466,7 @@
       </c>
       <c r="C28" s="20" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">STMT </v>
+        <v>STMT</v>
       </c>
       <c r="D28" s="23" t="str">
         <f t="shared" si="0"/>
@@ -7490,7 +7490,7 @@
       </c>
       <c r="C29" s="20" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">STMT </v>
+        <v>STMT</v>
       </c>
       <c r="D29" s="23" t="str">
         <f t="shared" si="0"/>
@@ -7514,7 +7514,7 @@
       </c>
       <c r="C30" s="20" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">STMT </v>
+        <v>STMT</v>
       </c>
       <c r="D30" s="23" t="str">
         <f t="shared" si="0"/>
@@ -7538,7 +7538,7 @@
       </c>
       <c r="C31" s="20" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">COND </v>
+        <v>COND</v>
       </c>
       <c r="D31" s="23" t="str">
         <f t="shared" si="0"/>
@@ -7562,7 +7562,7 @@
       </c>
       <c r="C32" s="20" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">COND </v>
+        <v>COND</v>
       </c>
       <c r="D32" s="23" t="str">
         <f t="shared" si="0"/>
@@ -7586,7 +7586,7 @@
       </c>
       <c r="C33" s="20" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">COND’ </v>
+        <v>COND’</v>
       </c>
       <c r="D33" s="23" t="str">
         <f t="shared" si="0"/>
@@ -7610,7 +7610,7 @@
       </c>
       <c r="C34" s="20" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">ELSE </v>
+        <v>ELSE</v>
       </c>
       <c r="D34" s="23" t="str">
         <f t="shared" si="0"/>
@@ -7634,7 +7634,7 @@
       </c>
       <c r="C35" s="20" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">ELSE </v>
+        <v>ELSE</v>
       </c>
       <c r="D35" s="23" t="str">
         <f t="shared" si="0"/>
@@ -7658,7 +7658,7 @@
       </c>
       <c r="C36" s="20" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">RETURN </v>
+        <v>RETURN</v>
       </c>
       <c r="D36" s="23" t="str">
         <f t="shared" si="0"/>
@@ -7682,7 +7682,7 @@
       </c>
       <c r="C37" s="20" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">CDECL </v>
+        <v>CDECL</v>
       </c>
       <c r="D37" s="23" t="str">
         <f t="shared" si="0"/>
@@ -7706,7 +7706,7 @@
       </c>
       <c r="C38" s="20" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">ODECL </v>
+        <v>ODECL</v>
       </c>
       <c r="D38" s="23" t="str">
         <f t="shared" si="0"/>
@@ -7730,7 +7730,7 @@
       </c>
       <c r="C39" s="20" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">ODECL </v>
+        <v>ODECL</v>
       </c>
       <c r="D39" s="23" t="str">
         <f t="shared" si="0"/>
@@ -7752,9 +7752,9 @@
       <c r="B40" s="21" t="s">
         <v>163</v>
       </c>
-      <c r="C40" s="21" t="str">
+      <c r="C40" s="20" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">ODECL </v>
+        <v>ODECL</v>
       </c>
       <c r="D40" s="24" t="str">
         <f t="shared" si="0"/>

</xml_diff>

<commit_message>
fix SLR_table.xlsx real fin
</commit_message>
<xml_diff>
--- a/SLR_table.xlsx
+++ b/SLR_table.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/eomchanwoo/CP_PROJECT/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F56CC85-DC5C-E144-896C-752D4326B95E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9561C65B-A2B7-0B45-B0FD-94807E8EDD90}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{DE6245F0-BCA7-4240-8F6E-8ABD7213D53C}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" activeTab="1" xr2:uid="{DE6245F0-BCA7-4240-8F6E-8ABD7213D53C}"/>
   </bookViews>
   <sheets>
     <sheet name="SLR_parse_table" sheetId="3" r:id="rId1"/>
@@ -2054,8 +2054,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C152AAA8-C259-2E48-8AC3-4CCFC4BB84A9}">
   <dimension ref="A1:AP88"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="L19" sqref="L19"/>
+    <sheetView topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18"/>
@@ -6791,8 +6791,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D1ECCCD-2683-9B43-BA07-36C0A247F203}">
   <dimension ref="A1:F41"/>
   <sheetViews>
-    <sheetView zoomScale="106" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView tabSelected="1" topLeftCell="A21" zoomScale="106" workbookViewId="0">
+      <selection activeCell="D32" sqref="D32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18"/>
@@ -7195,7 +7195,10 @@
         <f t="shared" si="3"/>
         <v>TERM</v>
       </c>
-      <c r="D17" s="14"/>
+      <c r="D17" s="14" t="str">
+        <f t="shared" si="0"/>
+        <v>FACTOR</v>
+      </c>
       <c r="E17" s="5">
         <f t="shared" ref="E17" si="4">IF(D17="''",0,LEN(D17)-LEN(SUBSTITUTE(D17," ",""))+1)</f>
         <v>1</v>
@@ -7758,7 +7761,7 @@
       </c>
     </row>
     <row r="41" spans="1:6" ht="19" thickBot="1">
-      <c r="A41" s="5">
+      <c r="A41" s="6">
         <v>39</v>
       </c>
       <c r="B41" s="12" t="s">

</xml_diff>

<commit_message>
fix SLR_table.xlsx real real fin
</commit_message>
<xml_diff>
--- a/SLR_table.xlsx
+++ b/SLR_table.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/eomchanwoo/CP_PROJECT/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9561C65B-A2B7-0B45-B0FD-94807E8EDD90}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28B4E71F-E4AF-1848-921C-DC7397F2D9A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" activeTab="1" xr2:uid="{DE6245F0-BCA7-4240-8F6E-8ABD7213D53C}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="14400" windowHeight="17500" activeTab="1" xr2:uid="{DE6245F0-BCA7-4240-8F6E-8ABD7213D53C}"/>
   </bookViews>
   <sheets>
     <sheet name="SLR_parse_table" sheetId="3" r:id="rId1"/>
@@ -1192,9 +1192,6 @@
     <t>CDECL -&gt; class id lbrace ODECL rbrace</t>
   </si>
   <si>
-    <t xml:space="preserve">ODECL -&gt; VDECL ODECL </t>
-  </si>
-  <si>
     <t>ODECL -&gt; FDECL ODECL</t>
   </si>
   <si>
@@ -1489,6 +1486,10 @@
   </si>
   <si>
     <t>FACTOR</t>
+  </si>
+  <si>
+    <t>ODECL -&gt; VDECL ODECL</t>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -2054,7 +2055,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C152AAA8-C259-2E48-8AC3-4CCFC4BB84A9}">
   <dimension ref="A1:AP88"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0">
+    <sheetView topLeftCell="N1" workbookViewId="0">
       <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
@@ -2066,7 +2067,7 @@
     <row r="1" spans="1:42" ht="19" thickBot="1">
       <c r="A1" s="19"/>
       <c r="B1" s="16" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C1" s="16" t="s">
         <v>0</v>
@@ -2150,10 +2151,10 @@
         <v>26</v>
       </c>
       <c r="AD1" s="16" t="s">
+        <v>172</v>
+      </c>
+      <c r="AE1" s="16" t="s">
         <v>173</v>
-      </c>
-      <c r="AE1" s="16" t="s">
-        <v>174</v>
       </c>
       <c r="AF1" s="16" t="s">
         <v>27</v>
@@ -3007,7 +3008,7 @@
       </c>
       <c r="L17" s="17"/>
       <c r="M17" s="17" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="N17" s="17"/>
       <c r="O17" s="17"/>
@@ -3129,7 +3130,7 @@
       <c r="M19" s="17"/>
       <c r="N19" s="17"/>
       <c r="O19" s="17" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="P19" s="17"/>
       <c r="Q19" s="17"/>
@@ -3520,7 +3521,7 @@
         <v>84</v>
       </c>
       <c r="J27" s="17" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="K27" s="17"/>
       <c r="L27" s="17" t="s">
@@ -3631,7 +3632,7 @@
       </c>
       <c r="L29" s="17"/>
       <c r="M29" s="17" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="N29" s="17"/>
       <c r="O29" s="17"/>
@@ -3795,7 +3796,7 @@
       <c r="M32" s="17"/>
       <c r="N32" s="17"/>
       <c r="O32" s="17" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="P32" s="17"/>
       <c r="Q32" s="17"/>
@@ -3845,7 +3846,7 @@
       <c r="M33" s="17"/>
       <c r="N33" s="17"/>
       <c r="O33" s="17" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="P33" s="17"/>
       <c r="Q33" s="17"/>
@@ -3901,7 +3902,7 @@
       <c r="M34" s="17"/>
       <c r="N34" s="17"/>
       <c r="O34" s="17" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="P34" s="17"/>
       <c r="Q34" s="17"/>
@@ -3954,7 +3955,7 @@
       <c r="L35" s="17"/>
       <c r="M35" s="17"/>
       <c r="N35" s="17" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="O35" s="17"/>
       <c r="P35" s="17"/>
@@ -4006,7 +4007,7 @@
       <c r="N36" s="17"/>
       <c r="O36" s="17"/>
       <c r="P36" s="17" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="Q36" s="17"/>
       <c r="R36" s="17"/>
@@ -4057,7 +4058,7 @@
       </c>
       <c r="L37" s="17"/>
       <c r="M37" s="17" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="N37" s="17"/>
       <c r="O37" s="17"/>
@@ -4113,7 +4114,7 @@
       </c>
       <c r="L38" s="17"/>
       <c r="M38" s="17" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="N38" s="17"/>
       <c r="O38" s="17"/>
@@ -4164,7 +4165,7 @@
       <c r="J39" s="17"/>
       <c r="K39" s="17"/>
       <c r="L39" s="17" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="M39" s="17"/>
       <c r="N39" s="17"/>
@@ -4464,7 +4465,7 @@
         <v>43</v>
       </c>
       <c r="B45" s="17" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C45" s="17"/>
       <c r="D45" s="17"/>
@@ -4524,7 +4525,7 @@
         <v>83</v>
       </c>
       <c r="J46" s="17" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="K46" s="17"/>
       <c r="L46" s="17" t="s">
@@ -4693,7 +4694,7 @@
       <c r="S49" s="17"/>
       <c r="T49" s="17"/>
       <c r="U49" s="17" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="V49" s="17"/>
       <c r="W49" s="1"/>
@@ -5151,7 +5152,7 @@
       <c r="M58" s="17"/>
       <c r="N58" s="17"/>
       <c r="O58" s="17" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="P58" s="17"/>
       <c r="Q58" s="17"/>
@@ -5207,7 +5208,7 @@
       </c>
       <c r="L59" s="17"/>
       <c r="M59" s="17" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="N59" s="17"/>
       <c r="O59" s="17"/>
@@ -5366,7 +5367,7 @@
       <c r="F62" s="17"/>
       <c r="G62" s="17"/>
       <c r="H62" s="17" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="I62" s="17"/>
       <c r="J62" s="17"/>
@@ -5418,7 +5419,7 @@
       <c r="F63" s="17"/>
       <c r="G63" s="17"/>
       <c r="H63" s="17" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="I63" s="17"/>
       <c r="J63" s="17"/>
@@ -5530,7 +5531,7 @@
       <c r="N65" s="17"/>
       <c r="O65" s="17"/>
       <c r="P65" s="17" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="Q65" s="17"/>
       <c r="R65" s="17"/>
@@ -5976,7 +5977,7 @@
       <c r="L74" s="17"/>
       <c r="M74" s="17"/>
       <c r="N74" s="17" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="O74" s="17"/>
       <c r="P74" s="17"/>
@@ -6018,7 +6019,7 @@
       <c r="F75" s="17"/>
       <c r="G75" s="17"/>
       <c r="H75" s="17" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="I75" s="17"/>
       <c r="J75" s="17"/>
@@ -6074,7 +6075,7 @@
       <c r="L76" s="17"/>
       <c r="M76" s="17"/>
       <c r="N76" s="17" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="O76" s="17"/>
       <c r="P76" s="17"/>
@@ -6353,7 +6354,7 @@
       <c r="M81" s="17"/>
       <c r="N81" s="17"/>
       <c r="O81" s="17" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="P81" s="17"/>
       <c r="Q81" s="17"/>
@@ -6578,7 +6579,7 @@
       <c r="L85" s="17"/>
       <c r="M85" s="17"/>
       <c r="N85" s="17" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="O85" s="17"/>
       <c r="P85" s="17"/>
@@ -6693,7 +6694,7 @@
       <c r="M87" s="17"/>
       <c r="N87" s="17"/>
       <c r="O87" s="17" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="P87" s="17"/>
       <c r="Q87" s="17"/>
@@ -6792,7 +6793,7 @@
   <dimension ref="A1:F41"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A21" zoomScale="106" workbookViewId="0">
-      <selection activeCell="D32" sqref="D32"/>
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18"/>
@@ -6806,22 +6807,22 @@
   <sheetData>
     <row r="1" spans="1:6" ht="19" thickBot="1">
       <c r="A1" s="9" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B1" s="9" t="s">
+        <v>140</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>138</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>139</v>
+      </c>
+      <c r="E1" s="9" t="s">
+        <v>145</v>
+      </c>
+      <c r="F1" s="9" t="s">
         <v>141</v>
-      </c>
-      <c r="C1" s="9" t="s">
-        <v>139</v>
-      </c>
-      <c r="D1" s="8" t="s">
-        <v>140</v>
-      </c>
-      <c r="E1" s="9" t="s">
-        <v>146</v>
-      </c>
-      <c r="F1" s="9" t="s">
-        <v>142</v>
       </c>
     </row>
     <row r="2" spans="1:6">
@@ -6829,7 +6830,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C2" s="10" t="str">
         <f>LEFT(B2,F2-1)</f>
@@ -6853,7 +6854,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="11" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C3" s="11" t="str">
         <f>LEFT(B3,F3-1)</f>
@@ -6925,7 +6926,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="11" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C6" s="11" t="str">
         <f t="shared" si="3"/>
@@ -7093,7 +7094,7 @@
         <v>11</v>
       </c>
       <c r="B13" s="11" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C13" s="11" t="str">
         <f t="shared" si="3"/>
@@ -7117,7 +7118,7 @@
         <v>12</v>
       </c>
       <c r="B14" s="11" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C14" s="11" t="str">
         <f t="shared" si="3"/>
@@ -7141,7 +7142,7 @@
         <v>13</v>
       </c>
       <c r="B15" s="11" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C15" s="11" t="str">
         <f t="shared" si="3"/>
@@ -7165,7 +7166,7 @@
         <v>14</v>
       </c>
       <c r="B16" s="11" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C16" s="11" t="str">
         <f t="shared" si="3"/>
@@ -7189,7 +7190,7 @@
         <v>15</v>
       </c>
       <c r="B17" s="11" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C17" s="11" t="str">
         <f t="shared" si="3"/>
@@ -7213,7 +7214,7 @@
         <v>16</v>
       </c>
       <c r="B18" s="11" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C18" s="11" t="str">
         <f t="shared" si="3"/>
@@ -7237,7 +7238,7 @@
         <v>17</v>
       </c>
       <c r="B19" s="11" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C19" s="11" t="str">
         <f t="shared" si="3"/>
@@ -7261,7 +7262,7 @@
         <v>18</v>
       </c>
       <c r="B20" s="11" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C20" s="11" t="str">
         <f t="shared" si="3"/>
@@ -7285,7 +7286,7 @@
         <v>19</v>
       </c>
       <c r="B21" s="11" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C21" s="11" t="str">
         <f t="shared" si="3"/>
@@ -7717,7 +7718,7 @@
         <v>37</v>
       </c>
       <c r="B39" s="11" t="s">
-        <v>135</v>
+        <v>174</v>
       </c>
       <c r="C39" s="11" t="str">
         <f t="shared" si="3"/>
@@ -7725,11 +7726,11 @@
       </c>
       <c r="D39" s="14" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">VDECL ODECL </v>
+        <v>VDECL ODECL</v>
       </c>
       <c r="E39" s="5">
         <f t="shared" si="1"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F39" s="5">
         <f t="shared" si="2"/>
@@ -7741,7 +7742,7 @@
         <v>38</v>
       </c>
       <c r="B40" s="11" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C40" s="11" t="str">
         <f t="shared" si="3"/>
@@ -7765,7 +7766,7 @@
         <v>39</v>
       </c>
       <c r="B41" s="12" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C41" s="12" t="str">
         <f t="shared" si="3"/>

</xml_diff>